<commit_message>
Complete 5MW strategic deployment and documentation updates
-   Updated create_financial_model.py for 5MW capacity, with .2M CapEx
-   Revised revenue projections to leverage GPU leasing + Bitcoin mining premium
-   Updated OpEx to 16K/month with bash.05 kWh power costs, and 5MW capacity
-   Updated README.md and assumptions.md files with the 5MW scope
-   Created Financing Options sheet.
-   Regenerated all charts.
</commit_message>
<xml_diff>
--- a/financial_model.xlsx
+++ b/financial_model.xlsx
@@ -6064,7 +6064,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>GridEdge Compute Center - 5MW Strategic Deployment</t>
+          <t>GridEdge Compute Center - Phase I 5MW Modular Launch</t>
         </is>
       </c>
       <c r="B1" t="inlineStr"/>
@@ -6088,7 +6088,7 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>6000000</v>
+        <v>6200000</v>
       </c>
     </row>
     <row r="5">

</xml_diff>